<commit_message>
vendor tables & controller
</commit_message>
<xml_diff>
--- a/documents/Milestones.xlsx
+++ b/documents/Milestones.xlsx
@@ -1,122 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\bookApp\documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" xr2:uid="{D0C57D63-1129-4792-91B8-CFF17D3F07DF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
     <sheet name="Restourent data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Kaushal Mehra</author>
-  </authors>
-  <commentList>
-    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{1BA44713-4B69-41B1-BC9E-07DA7DE1934A}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Kaushal Mehra:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-0=draft
-1=review
-2=publish
-3=decline
-4=delete</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B61" authorId="0" shapeId="0" xr:uid="{56019ECC-5AC5-40FA-87D3-F311648A1818}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Kaushal Mehra:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-0=new
-1=process
-2=complete
-3=cancle</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B62" authorId="0" shapeId="0" xr:uid="{9A9B5242-437B-40FD-A3CD-087039BD955C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Kaushal Mehra:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-0=not received
-1= received
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="115">
   <si>
     <t>products</t>
   </si>
@@ -283,9 +188,6 @@
     <t>display_name</t>
   </si>
   <si>
-    <t>business_description</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -461,13 +363,16 @@
   </si>
   <si>
     <t>wishlists</t>
+  </si>
+  <si>
+    <t>delete_at</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,32 +393,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -610,8 +489,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -619,8 +498,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -682,7 +561,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -734,7 +613,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -928,21 +807,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7201DD73-D7EE-40B0-96A5-18F2B4E4B774}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -955,25 +834,25 @@
     <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="2:12">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="12"/>
+      <c r="E2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="H2" s="9" t="s">
+      <c r="F2" s="12"/>
+      <c r="H2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="9"/>
+      <c r="I2" s="12"/>
       <c r="K2" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L2" s="11"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -999,7 +878,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1025,7 +904,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1047,9 +926,9 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -1065,7 +944,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1081,7 +960,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1089,7 +968,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1097,19 +976,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="2:12">
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1123,13 +1002,13 @@
         <v>16</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I11" s="11"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>16</v>
@@ -1147,7 +1026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1167,7 +1046,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12">
       <c r="B14" s="1" t="s">
         <v>37</v>
       </c>
@@ -1175,7 +1054,7 @@
         <v>16</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>14</v>
@@ -1187,7 +1066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1203,9 +1082,9 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12">
       <c r="B16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>16</v>
@@ -1215,19 +1094,19 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12">
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12">
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12">
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -1240,25 +1119,25 @@
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+    <row r="22" spans="2:12">
+      <c r="B22" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="E22" s="9" t="s">
+      <c r="C22" s="12"/>
+      <c r="E22" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="9"/>
+      <c r="F22" s="12"/>
       <c r="H22" s="5" t="s">
         <v>48</v>
       </c>
       <c r="I22" s="6"/>
-      <c r="K22" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="L22" s="9"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K22" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="L22" s="12"/>
+    </row>
+    <row r="23" spans="2:12">
       <c r="B23" s="1" t="s">
         <v>1</v>
       </c>
@@ -1272,7 +1151,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12">
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1281,16 +1160,15 @@
         <v>37</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="H24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I24" s="1"/>
-      <c r="K24" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="L24" s="9"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L24" s="12"/>
+    </row>
+    <row r="25" spans="2:12">
       <c r="B25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1300,11 +1178,11 @@
       </c>
       <c r="F25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12">
       <c r="B26" s="3" t="s">
         <v>36</v>
       </c>
@@ -1314,15 +1192,15 @@
       </c>
       <c r="F26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I26" s="1"/>
-      <c r="K26" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="L26" s="9"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K26" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="L26" s="12"/>
+    </row>
+    <row r="27" spans="2:12">
       <c r="B27" s="1" t="s">
         <v>32</v>
       </c>
@@ -1332,11 +1210,11 @@
       </c>
       <c r="F27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12">
       <c r="B28" s="1" t="s">
         <v>33</v>
       </c>
@@ -1346,11 +1224,11 @@
       </c>
       <c r="F28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12">
       <c r="B29" s="2" t="s">
         <v>11</v>
       </c>
@@ -1360,11 +1238,11 @@
       </c>
       <c r="F29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12">
       <c r="B30" s="2" t="s">
         <v>12</v>
       </c>
@@ -1373,69 +1251,69 @@
         <v>43</v>
       </c>
       <c r="F30" s="1"/>
-      <c r="H30" s="2" t="s">
-        <v>11</v>
+      <c r="H30" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12">
       <c r="E31" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F31" s="1"/>
       <c r="H31" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12">
       <c r="E32" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="2:9">
       <c r="B33" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C33" s="4"/>
       <c r="E33" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F33" s="1"/>
-      <c r="H33" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I33" s="6"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:9">
       <c r="B34" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F34" s="1"/>
-      <c r="H34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="2:9">
       <c r="B35" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C35" s="1"/>
       <c r="E35" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" s="3" t="s">
         <v>34</v>
       </c>
@@ -1444,14 +1322,13 @@
         <v>11</v>
       </c>
       <c r="F36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
       <c r="B37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C37" s="1"/>
       <c r="E37" s="2" t="s">
@@ -1459,94 +1336,107 @@
       </c>
       <c r="F37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9">
       <c r="B38" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="2:9">
       <c r="B39" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="2:9">
       <c r="B40" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C40" s="1"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9">
       <c r="B43" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C43" s="6"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9">
       <c r="B44" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9">
       <c r="B45" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9">
       <c r="B46" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9">
       <c r="B47" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9">
       <c r="B48" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12">
       <c r="B49" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12">
       <c r="B50" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12">
       <c r="B51" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
+    <row r="52" spans="2:12">
+      <c r="B52" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12">
+      <c r="B53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="2:12">
+      <c r="B54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C53" s="1"/>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55" spans="2:12">
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
@@ -1559,21 +1449,21 @@
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B57" s="9" t="s">
+    <row r="57" spans="2:12">
+      <c r="B57" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C57" s="12"/>
+      <c r="E57" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F57" s="12"/>
+      <c r="H57" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C57" s="9"/>
-      <c r="E57" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="F57" s="9"/>
-      <c r="H57" s="10" t="s">
-        <v>93</v>
-      </c>
       <c r="I57" s="11"/>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12">
       <c r="B58" s="1" t="s">
         <v>1</v>
       </c>
@@ -1587,13 +1477,13 @@
       </c>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12">
       <c r="B59" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F59" s="1"/>
       <c r="H59" s="1" t="s">
@@ -1601,55 +1491,55 @@
       </c>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12">
       <c r="B60" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C60" s="12"/>
+        <v>97</v>
+      </c>
+      <c r="C60" s="9"/>
       <c r="E60" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F60" s="12"/>
+      <c r="F60" s="9"/>
       <c r="H60" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12">
       <c r="B61" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C61" s="1"/>
       <c r="E61" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F61" s="1"/>
       <c r="H61" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12">
       <c r="B62" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C62" s="1"/>
       <c r="E62" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F62" s="1"/>
       <c r="H62" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12">
       <c r="B63" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C63" s="1"/>
       <c r="E63" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F63" s="1"/>
       <c r="H63" s="2" t="s">
@@ -1657,13 +1547,13 @@
       </c>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:12">
       <c r="B64" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C64" s="1"/>
       <c r="E64" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F64" s="1"/>
       <c r="H64" s="2" t="s">
@@ -1671,37 +1561,37 @@
       </c>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9">
       <c r="B65" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C65" s="1"/>
       <c r="E65" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9">
       <c r="B66" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C66" s="1"/>
       <c r="E66" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F66" s="1"/>
       <c r="H66" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I66" s="11"/>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9">
       <c r="B67" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C67" s="1"/>
       <c r="E67" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F67" s="1"/>
       <c r="H67" s="1" t="s">
@@ -1709,9 +1599,9 @@
       </c>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9">
       <c r="B68" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C68" s="1"/>
       <c r="E68" s="2" t="s">
@@ -1723,9 +1613,9 @@
       </c>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9">
       <c r="B69" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C69" s="1"/>
       <c r="E69" s="2" t="s">
@@ -1737,17 +1627,17 @@
       </c>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9">
       <c r="B70" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C70" s="1"/>
       <c r="H70" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9">
       <c r="B71" s="2" t="s">
         <v>12</v>
       </c>
@@ -1757,7 +1647,7 @@
       </c>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9">
       <c r="H72" s="2" t="s">
         <v>12</v>
       </c>
@@ -1765,13 +1655,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E10:F10"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="B57:C57"/>
@@ -1780,22 +1663,28 @@
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="E22:F22"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F042A85D-680B-4AE1-86A1-90F0FFCEE1E9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -1803,12 +1692,12 @@
     <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
         <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
       </c>
       <c r="C2">
         <v>7737185555</v>
@@ -1817,15 +1706,15 @@
         <v>9602691301</v>
       </c>
       <c r="E2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" t="s">
-        <v>72</v>
       </c>
       <c r="C3">
         <v>9783341410</v>
@@ -1834,12 +1723,12 @@
         <v>9610015000</v>
       </c>
       <c r="E3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>74</v>
       </c>
       <c r="C4">
         <v>9829809969</v>
@@ -1848,12 +1737,12 @@
         <v>9829809699</v>
       </c>
       <c r="E4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>76</v>
       </c>
       <c r="C5">
         <v>9602067770</v>
@@ -1862,26 +1751,26 @@
         <v>8107771105</v>
       </c>
       <c r="E5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>78</v>
-      </c>
-      <c r="B6" t="s">
-        <v>79</v>
       </c>
       <c r="C6">
         <v>9873878528</v>
       </c>
       <c r="E6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>81</v>
       </c>
       <c r="C7">
         <v>9602587855</v>
@@ -1890,37 +1779,37 @@
         <v>7737160178</v>
       </c>
       <c r="E7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>83</v>
-      </c>
-      <c r="B8" t="s">
-        <v>84</v>
       </c>
       <c r="C8">
         <v>8290876000</v>
       </c>
       <c r="E8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>86</v>
       </c>
       <c r="C9">
         <v>9414557404</v>
       </c>
       <c r="E9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>